<commit_message>
switch to essd data
</commit_message>
<xml_diff>
--- a/R/Analysis and figures for ESSD paper/UNFCCC reports.xlsx
+++ b/R/Analysis and figures for ESSD paper/UNFCCC reports.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banl\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamw\Documents\SpiderOak Hive\Work\Projects\AR6-Emissions-trends-and-drivers\R\Analysis and figures for ESSD paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5112" windowHeight="324"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5115" windowHeight="330"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -410,9 +410,6 @@
     <t>Mexico</t>
   </si>
   <si>
-    <t>Micornesia</t>
-  </si>
-  <si>
     <t>Mongolia</t>
   </si>
   <si>
@@ -623,9 +620,6 @@
     <t>Uzbekistan</t>
   </si>
   <si>
-    <t>Vanatu</t>
-  </si>
-  <si>
     <t>Venezuela</t>
   </si>
   <si>
@@ -806,9 +800,6 @@
     <t>Turkey</t>
   </si>
   <si>
-    <t>Urkaine</t>
-  </si>
-  <si>
     <t>United Kingdom</t>
   </si>
   <si>
@@ -822,6 +813,15 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>Micronesia</t>
   </si>
 </sst>
 </file>
@@ -1146,24 +1146,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J169" sqref="J169"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1192,13 +1192,13 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1241,10 +1241,10 @@
         <v>1990</v>
       </c>
       <c r="I3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1278,10 +1278,10 @@
         <v>1990</v>
       </c>
       <c r="I5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1376,10 +1376,10 @@
         <v>1990</v>
       </c>
       <c r="I9" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
@@ -1561,10 +1561,10 @@
         <v>1990</v>
       </c>
       <c r="I19" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>36</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>41</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>42</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>43</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>44</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>48</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>50</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>51</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>52</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>53</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>54</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>55</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>56</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>62</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>64</v>
       </c>
@@ -1972,10 +1972,10 @@
         <v>1994</v>
       </c>
       <c r="I40" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>65</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>66</v>
       </c>
@@ -2003,10 +2003,10 @@
         <v>1994</v>
       </c>
       <c r="I42" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>67</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>68</v>
       </c>
@@ -2046,13 +2046,13 @@
         <v>42927</v>
       </c>
       <c r="G44" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H44" s="2">
         <v>1990</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>69</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>70</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>71</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>72</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>73</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>74</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>75</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>76</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>77</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>78</v>
       </c>
@@ -2231,10 +2231,10 @@
         <v>1980</v>
       </c>
       <c r="I54" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>79</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>80</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>81</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>82</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>83</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>84</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>85</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>86</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>87</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>88</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>89</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>90</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>91</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>92</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>93</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>94</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>95</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>96</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>97</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>98</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>99</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>100</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>101</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>102</v>
       </c>
@@ -2693,12 +2693,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>117</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>118</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>120</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>121</v>
       </c>
@@ -2772,10 +2772,10 @@
         <v>1994</v>
       </c>
       <c r="I83" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>122</v>
       </c>
@@ -2789,10 +2789,10 @@
         <v>1995</v>
       </c>
       <c r="I84" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>123</v>
       </c>
@@ -2806,10 +2806,10 @@
         <v>1990</v>
       </c>
       <c r="I85" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>124</v>
       </c>
@@ -2820,13 +2820,13 @@
         <v>2010</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J86" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>125</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>126</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>127</v>
       </c>
@@ -2904,12 +2904,12 @@
         <v>1990</v>
       </c>
       <c r="I89" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>128</v>
+        <v>265</v>
       </c>
       <c r="D90" s="1">
         <v>42320</v>
@@ -2921,9 +2921,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B91" s="1">
         <v>42977</v>
@@ -2950,9 +2950,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B92" s="1">
         <v>43588</v>
@@ -2973,9 +2973,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B93" s="1">
         <v>43830</v>
@@ -2993,9 +2993,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D94" s="1">
         <v>38870</v>
@@ -3007,9 +3007,9 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D95" s="1">
         <v>41269</v>
@@ -3021,9 +3021,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B96" s="1">
         <v>44245</v>
@@ -3047,12 +3047,12 @@
         <v>1990</v>
       </c>
       <c r="I96" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D97" s="1">
         <v>42095</v>
@@ -3064,23 +3064,23 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D98" s="1">
         <v>42342</v>
       </c>
       <c r="E98" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D99" s="1">
         <v>43342</v>
@@ -3092,9 +3092,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D100" s="1">
         <v>42739</v>
@@ -3106,12 +3106,12 @@
         <v>1997</v>
       </c>
       <c r="I100" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B101" s="1">
         <v>43176</v>
@@ -3129,12 +3129,12 @@
         <v>1988</v>
       </c>
       <c r="I101" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D102" s="1">
         <v>42630</v>
@@ -3146,12 +3146,12 @@
         <v>1994</v>
       </c>
       <c r="I102" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B103" s="1">
         <v>43822</v>
@@ -3169,9 +3169,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D104" s="1">
         <v>43717</v>
@@ -3183,9 +3183,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D105" s="1">
         <v>43703</v>
@@ -3197,12 +3197,12 @@
         <v>1994</v>
       </c>
       <c r="I105" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B106" s="1">
         <v>44282</v>
@@ -3220,12 +3220,12 @@
         <v>1994</v>
       </c>
       <c r="I106" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B107" s="1">
         <v>43572</v>
@@ -3243,12 +3243,12 @@
         <v>1994</v>
       </c>
       <c r="I107" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B108" s="1">
         <v>43461</v>
@@ -3266,12 +3266,12 @@
         <v>1990</v>
       </c>
       <c r="I108" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B109" s="1">
         <v>43816</v>
@@ -3295,9 +3295,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D110" s="1">
         <v>42002</v>
@@ -3309,9 +3309,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D111" s="1">
         <v>40714</v>
@@ -3323,9 +3323,9 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B112" s="1">
         <v>43799</v>
@@ -3346,9 +3346,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B113" s="1">
         <v>43574</v>
@@ -3375,9 +3375,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D114" s="1">
         <v>43423</v>
@@ -3389,12 +3389,12 @@
         <v>1990</v>
       </c>
       <c r="I114" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D115" s="1">
         <v>42440</v>
@@ -3406,12 +3406,12 @@
         <v>1994</v>
       </c>
       <c r="I115" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D116" s="1">
         <v>42991</v>
@@ -3423,9 +3423,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D117" s="1">
         <v>42489</v>
@@ -3437,9 +3437,9 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D118" s="1">
         <v>40343</v>
@@ -3451,12 +3451,12 @@
         <v>1994</v>
       </c>
       <c r="I118" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D119" s="1">
         <v>41302</v>
@@ -3468,9 +3468,9 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D120" s="1">
         <v>43742</v>
@@ -3482,9 +3482,9 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B121" s="1">
         <v>43193</v>
@@ -3502,9 +3502,9 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D122" s="1">
         <v>42377</v>
@@ -3516,9 +3516,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B123" s="1">
         <v>42457</v>
@@ -3536,12 +3536,12 @@
         <v>1990</v>
       </c>
       <c r="I123" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D124" s="1">
         <v>41378</v>
@@ -3553,9 +3553,9 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D125" s="1">
         <v>43163</v>
@@ -3567,9 +3567,9 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B126" s="1">
         <v>44192</v>
@@ -3590,9 +3590,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D127" s="1">
         <v>42992</v>
@@ -3604,9 +3604,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D128" s="1">
         <v>43484</v>
@@ -3618,12 +3618,12 @@
         <v>2000</v>
       </c>
       <c r="I128" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B129" s="1">
         <v>43621</v>
@@ -3647,12 +3647,12 @@
         <v>1990</v>
       </c>
       <c r="I129" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D130" s="1">
         <v>43696</v>
@@ -3664,12 +3664,12 @@
         <v>2012</v>
       </c>
       <c r="I130" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D131" s="1">
         <v>40984</v>
@@ -3681,9 +3681,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D132" s="1">
         <v>42685</v>
@@ -3695,9 +3695,9 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D133" s="1">
         <v>41592</v>
@@ -3709,9 +3709,9 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D134" s="1">
         <v>42444</v>
@@ -3723,9 +3723,9 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D135" s="1">
         <v>40541</v>
@@ -3737,12 +3737,12 @@
         <v>1994</v>
       </c>
       <c r="I135" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B136" s="1">
         <v>43664</v>
@@ -3763,9 +3763,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B137" s="1">
         <v>44190</v>
@@ -3786,9 +3786,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B138" s="1">
         <v>43164</v>
@@ -3815,9 +3815,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D139" s="1">
         <v>44152</v>
@@ -3832,9 +3832,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B140" s="1">
         <v>43005</v>
@@ -3858,9 +3858,9 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D141" s="1">
         <v>43873</v>
@@ -3872,9 +3872,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D142" s="1">
         <v>41585</v>
@@ -3886,9 +3886,9 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B143" s="1">
         <v>42735</v>
@@ -3906,12 +3906,12 @@
         <v>1994</v>
       </c>
       <c r="I143" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D144" s="1">
         <v>42374</v>
@@ -3923,9 +3923,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D145" s="1">
         <v>43178</v>
@@ -3937,9 +3937,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B146" s="1">
         <v>43739</v>
@@ -3957,9 +3957,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D147" s="1">
         <v>43486</v>
@@ -3971,9 +3971,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D148" s="1">
         <v>42317</v>
@@ -3985,9 +3985,9 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B149" s="1">
         <v>43830</v>
@@ -4005,9 +4005,9 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D150" s="1">
         <v>42787</v>
@@ -4019,9 +4019,9 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>199</v>
+        <v>264</v>
       </c>
       <c r="D151" s="1">
         <v>44277</v>
@@ -4033,12 +4033,12 @@
         <v>1994</v>
       </c>
       <c r="I151" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D152" s="1">
         <v>43125</v>
@@ -4050,9 +4050,9 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B153" s="1">
         <v>44302</v>
@@ -4076,9 +4076,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B154" s="1">
         <v>43375</v>
@@ -4096,15 +4096,15 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B155" s="1">
         <v>44172</v>
       </c>
       <c r="C155" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D155" s="1">
         <v>44098</v>
@@ -4116,9 +4116,9 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D156" s="1">
         <v>42747</v>
@@ -4130,348 +4130,348 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K157" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="K158" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="K157" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A158" s="3" t="s">
+      <c r="K159" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="K158" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A159" s="3" t="s">
+      <c r="K160" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="K159" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A160" s="3" t="s">
+      <c r="K161" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="K160" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A161" s="3" t="s">
+      <c r="K162" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="K161" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A162" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="K162" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A163" s="3" t="s">
-        <v>229</v>
-      </c>
       <c r="K163" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>61</v>
       </c>
       <c r="K164" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="K165" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="K166" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="K165" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A166" s="3" t="s">
+      <c r="K167" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="K166" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A167" s="3" t="s">
+      <c r="K168" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="K167" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A168" s="3" t="s">
+      <c r="K169" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="K168" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A169" s="3" t="s">
+      <c r="K170" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="K169" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A170" s="3" t="s">
+      <c r="K171" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="K170" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A171" s="3" t="s">
+      <c r="K172" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="K171" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A172" s="3" t="s">
+      <c r="K173" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="K172" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A173" s="3" t="s">
+      <c r="K174" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="K173" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A174" s="3" t="s">
+      <c r="K175" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="K174" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A175" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="K175" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A176" s="3" t="s">
-        <v>241</v>
-      </c>
       <c r="K176" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>94</v>
       </c>
       <c r="K177" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="K178" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="K179" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A180" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="K178" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A179" s="3" t="s">
+      <c r="K180" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="K179" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A180" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="K180" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A181" s="3" t="s">
-        <v>245</v>
-      </c>
       <c r="K181" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>123</v>
       </c>
       <c r="K182" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="K183" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="K184" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="K183" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A184" s="3" t="s">
+      <c r="K185" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="K184" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A185" s="3" t="s">
+      <c r="K186" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="K185" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A186" s="3" t="s">
+      <c r="K187" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="K186" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A187" s="3" t="s">
+      <c r="K188" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="K187" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A188" s="3" t="s">
+      <c r="K189" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="K188" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A189" s="3" t="s">
+      <c r="K190" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="K189" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A190" s="3" t="s">
+      <c r="K191" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="K190" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A191" s="3" t="s">
+      <c r="K192" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="K191" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A192" s="3" t="s">
+      <c r="K193" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="K192" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A193" s="3" t="s">
+      <c r="K194" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="K193" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A194" s="3" t="s">
+      <c r="K195" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K194" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A195" s="3" t="s">
+      <c r="K196" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="K197" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="K195" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A196" s="3" t="s">
+      <c r="K198" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A199" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="K196" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A197" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="K197" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A198" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="K198" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A199" s="3" t="s">
+      <c r="K199" t="s">
         <v>262</v>
-      </c>
-      <c r="K199" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>